<commit_message>
modifying inline commands ignore for now
</commit_message>
<xml_diff>
--- a/PlanPrepareProcess/Testing Plans/df.xlsx
+++ b/PlanPrepareProcess/Testing Plans/df.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edwin\Desktop\OT2-DOE\PlanPrepareProcess\Prepare\Testing Plans\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edwin\Desktop\OT2-DOE\PlanPrepareProcess\Testing Plans\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -437,7 +437,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>